<commit_message>
updated tw ettv source
</commit_message>
<xml_diff>
--- a/channels.xlsx
+++ b/channels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\shen_workplace\github\KimShenGod.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E09C86D-F4B9-4CB8-B6C0-4586293168E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCD94A7-7C66-460B-AE76-087587CD6C18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HK" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="106">
   <si>
     <t>序号</t>
   </si>
@@ -155,13 +155,196 @@
     <t>http://50.7.234.10:8278/rhk31_twn/playlist.m3u8?tid=MA6A6225600662256006&amp;ct=19249&amp;tsum=7b0adccccff4fded44e906e9d848ee35</t>
   </si>
   <si>
-    <t>https://stream1.freetv.fun/61c9519e70540235a366f9e5c9f5b4e95ad06ee6cb1edc8647cb99dd28c28960.m3u8</t>
-  </si>
-  <si>
     <t>https://epg.pw/stream/1496043c9019ec1e6c21f1257e1f303b901a1f4effc143fb7da3c19cc4de0ecc.m3u8</t>
   </si>
   <si>
     <t>http://php.jdshipin.com:8880/TVOD/iptv.php?id=j2</t>
+  </si>
+  <si>
+    <t>https://epg.pw/stream/61c9519e70540235a366f9e5c9f5b4e95ad06ee6cb1edc8647cb99dd28c28960.m3u8</t>
+  </si>
+  <si>
+    <t>TVBS</t>
+  </si>
+  <si>
+    <t>华视</t>
+  </si>
+  <si>
+    <t>中视</t>
+  </si>
+  <si>
+    <t>民视</t>
+  </si>
+  <si>
+    <t>台视</t>
+  </si>
+  <si>
+    <t>公视</t>
+  </si>
+  <si>
+    <t>三立</t>
+  </si>
+  <si>
+    <t>中天</t>
+  </si>
+  <si>
+    <t>八大</t>
+  </si>
+  <si>
+    <t>ELTA</t>
+  </si>
+  <si>
+    <t>龙华</t>
+  </si>
+  <si>
+    <t>龙祥</t>
+  </si>
+  <si>
+    <t>纬来</t>
+  </si>
+  <si>
+    <t>靖天</t>
+  </si>
+  <si>
+    <t>靖洋</t>
+  </si>
+  <si>
+    <t>EYE</t>
+  </si>
+  <si>
+    <t>大爱</t>
+  </si>
+  <si>
+    <t>壹新闻</t>
+  </si>
+  <si>
+    <t>壹电影</t>
+  </si>
+  <si>
+    <t>年代</t>
+  </si>
+  <si>
+    <t>非凡</t>
+  </si>
+  <si>
+    <t>镜新闻</t>
+  </si>
+  <si>
+    <t>寰宇</t>
+  </si>
+  <si>
+    <t>博斯</t>
+  </si>
+  <si>
+    <t>国会</t>
+  </si>
+  <si>
+    <t>TVBS HD</t>
+  </si>
+  <si>
+    <t>TVBS NEWS</t>
+  </si>
+  <si>
+    <t>TVBS 新闻</t>
+  </si>
+  <si>
+    <t>TVBS亚洲</t>
+  </si>
+  <si>
+    <t>TVBS欢乐</t>
+  </si>
+  <si>
+    <t>TVBS精采</t>
+  </si>
+  <si>
+    <t>东森新闻</t>
+  </si>
+  <si>
+    <t>东森超视</t>
+  </si>
+  <si>
+    <t>东森美洲</t>
+  </si>
+  <si>
+    <t>东森美洲卫视</t>
+  </si>
+  <si>
+    <t>东森亚洲</t>
+  </si>
+  <si>
+    <t>东森综合</t>
+  </si>
+  <si>
+    <t>东森洋片</t>
+  </si>
+  <si>
+    <t>东森电影</t>
+  </si>
+  <si>
+    <t>东森戏剧</t>
+  </si>
+  <si>
+    <t>东森财经新闻</t>
+  </si>
+  <si>
+    <t>东森幼幼</t>
+  </si>
+  <si>
+    <t>东森幼幼HD</t>
+  </si>
+  <si>
+    <t>http://37.27.111.214:8080/live/23/hls.m3u8</t>
+  </si>
+  <si>
+    <t>http://61.221.215.25:8800/hls/9/index.m3u8</t>
+  </si>
+  <si>
+    <t>http://211.72.65.236:8574/.m3u8</t>
+  </si>
+  <si>
+    <t>http://37.27.111.214:8080/live/24/hls.m3u8</t>
+  </si>
+  <si>
+    <t>https://epg.pw/stream/c88adc69fe22cc05c7ff2984ad14db99f461e6dda12687cb7bbaf5e03a357a38.m3u8</t>
+  </si>
+  <si>
+    <t>http://38.64.72.148:80/hls/modn/list/4005/chunklist1.m3u8</t>
+  </si>
+  <si>
+    <t>TVBS台剧</t>
+  </si>
+  <si>
+    <t>TVBS综艺</t>
+  </si>
+  <si>
+    <t>http://37.27.111.214:8080/live/20/hls.m3u8</t>
+  </si>
+  <si>
+    <t>https://epg.pw/stream/41fd1dc90b335e2c39f811e013a8bc45d966113d4b326afb8bed450591629da1.m3u8</t>
+  </si>
+  <si>
+    <t>https://epg.pw/stream/568e26b29122e84e3527b97eca553332274777bdf39873fb234fb6581a3f6a59.m3u8</t>
+  </si>
+  <si>
+    <t>http://50.7.234.10:8278/j2_twn/playlist.m3u8?tid=MFCF3274854132748541&amp;ct=19254&amp;tsum=699466c18aac56202ad1d2843fd21032</t>
+  </si>
+  <si>
+    <t>http://50.7.234.10:8278/ettvmovie/playlist.m3u8?tid=MBDB9268852192688521&amp;ct=19254&amp;tsum=7514b50ebc2e4b06f2e402578d0ac996</t>
+  </si>
+  <si>
+    <t>http://50.7.234.10:8278/ettvdrama/playlist.m3u8?tid=MA2A9945921599459215&amp;ct=19249&amp;tsum=c9097ecdf4a17c0922196dbf04b0c6e7</t>
+  </si>
+  <si>
+    <t>http://50.7.234.10:8278/ettvcaijing_twn/playlist.m3u8?tid=MD5D9010164090101640&amp;ct=19225&amp;tsum=cc229773020f89af853b23d81e0e6371</t>
+  </si>
+  <si>
+    <t>http://50.7.234.10:8278/ettvzhonghe/playlist.m3u8?tid=MC4C1214674912146749&amp;ct=19254&amp;tsum=9b96a50ba99dca1a02a27b05a6fb4b0d</t>
+  </si>
+  <si>
+    <t>https://epg.pw/stream/bab8065e884e2bdc304409c9cad21b27e7ecfe42e7c3476ffa0ef5a9165647bd.m3u8</t>
+  </si>
+  <si>
+    <t>东森超视34.5</t>
   </si>
 </sst>
 </file>
@@ -206,9 +389,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -492,15 +681,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.5546875" customWidth="1"/>
     <col min="5" max="5" width="90.109375" customWidth="1"/>
-    <col min="6" max="6" width="37.44140625" customWidth="1"/>
+    <col min="6" max="6" width="37.44140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="50.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -520,7 +709,7 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
@@ -605,12 +794,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -638,7 +830,7 @@
         <v>18</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
@@ -646,7 +838,7 @@
         <v>19</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
@@ -706,6 +898,7 @@
     <hyperlink ref="E20" r:id="rId9" xr:uid="{A6E0BB72-BEB2-431F-859D-C7F553410A5D}"/>
     <hyperlink ref="E19" r:id="rId10" xr:uid="{84ED8DF0-D977-4704-A2D5-1810B455E63B}"/>
     <hyperlink ref="E14" r:id="rId11" xr:uid="{7730D9D3-1B8A-4C5F-A98C-B439B9B7B4FD}"/>
+    <hyperlink ref="F14" r:id="rId12" xr:uid="{9E9C4A73-ED97-4F41-B9DA-523774C4961C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -713,14 +906,313 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A588FBF-255C-4CC0-BFE2-40A1B22C0CA5}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="65.77734375" customWidth="1"/>
+    <col min="5" max="5" width="46.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{8CE6FCE6-87C8-438C-90F5-24097D41C396}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{EAD96624-B978-4D87-876F-2AB911407755}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{F068507F-A179-43F3-A701-2EAC21CDF5F5}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{094B5F37-5C61-41AF-98AA-C7815D254731}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{48434FE3-F406-413D-83A8-9CFBCD10CDD6}"/>
+    <hyperlink ref="D2" r:id="rId6" xr:uid="{93EA0B14-D55A-4DF6-9CBF-87DC080E8D24}"/>
+    <hyperlink ref="D11" r:id="rId7" xr:uid="{7E7C5CC5-1B45-474E-8243-1BF7E82C3C04}"/>
+    <hyperlink ref="D14" r:id="rId8" xr:uid="{505E2747-0AB1-48F8-9554-425FAD8F2CE4}"/>
+    <hyperlink ref="D15" r:id="rId9" xr:uid="{4729FAB0-63F9-4CAB-983B-6B11750C7899}"/>
+    <hyperlink ref="D19" r:id="rId10" xr:uid="{08CB9735-DCE3-438E-9289-9F3B81E6EA02}"/>
+    <hyperlink ref="D20" r:id="rId11" xr:uid="{E3D86602-8147-4989-A0E2-E6FA66B31E40}"/>
+    <hyperlink ref="D21" r:id="rId12" xr:uid="{3B81DEDD-6D9F-4A45-9575-AE8A5F7515F2}"/>
+    <hyperlink ref="D17" r:id="rId13" xr:uid="{73698551-E644-4E9C-A125-B1134020A15C}"/>
+    <hyperlink ref="D13" r:id="rId14" xr:uid="{8D8AD8A1-3727-4433-91A2-54816EE6D726}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated TVBS serial channes
</commit_message>
<xml_diff>
--- a/channels.xlsx
+++ b/channels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\shen_workplace\github\KimShenGod.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCD94A7-7C66-460B-AE76-087587CD6C18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E29152-CBB6-42B6-8477-0FFF4991E0E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
   <si>
     <t>序号</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>东森超视34.5</t>
+  </si>
+  <si>
+    <t>https://aktv.top/AKTV/live/aktv/null-2/AKTV.m3u8</t>
+  </si>
+  <si>
+    <t>https://aktv.top/AKTV/live/aktv/null-1/AKTV.m3u8</t>
   </si>
 </sst>
 </file>
@@ -681,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,6 +745,9 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -818,6 +827,9 @@
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>15</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -899,6 +911,8 @@
     <hyperlink ref="E19" r:id="rId10" xr:uid="{84ED8DF0-D977-4704-A2D5-1810B455E63B}"/>
     <hyperlink ref="E14" r:id="rId11" xr:uid="{7730D9D3-1B8A-4C5F-A98C-B439B9B7B4FD}"/>
     <hyperlink ref="F14" r:id="rId12" xr:uid="{9E9C4A73-ED97-4F41-B9DA-523774C4961C}"/>
+    <hyperlink ref="E4" r:id="rId13" xr:uid="{DC5A7FEF-4339-473F-AD3A-39C9948877F1}"/>
+    <hyperlink ref="E17" r:id="rId14" xr:uid="{80ADBE0D-1133-4750-AB9A-5294D47FA043}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -909,7 +923,7 @@
   <dimension ref="B1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>